<commit_message>
Finish visualizaiton by geography
</commit_message>
<xml_diff>
--- a/project-intl-flight-tracking/data-sources/geographic/crude-price-by-region.xlsx
+++ b/project-intl-flight-tracking/data-sources/geographic/crude-price-by-region.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sharonhe/Documents/data-visualizations/project-intl-flight-tracking/data-sources/geographic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5979A65C-F56A-9B4E-AB44-17E1F49E2849}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1EF60A-538D-224B-B420-EF2C2731D647}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15480" yWindow="1960" windowWidth="27640" windowHeight="16040" xr2:uid="{5F7A381C-8C5E-4C47-B42D-B9FEE3CD53A3}"/>
   </bookViews>
@@ -33,153 +33,159 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
-  <si>
-    <t>Alabama</t>
-  </si>
-  <si>
-    <t>Alaska</t>
-  </si>
-  <si>
-    <t>Arizona</t>
-  </si>
-  <si>
-    <t>Arkansas</t>
-  </si>
-  <si>
-    <t>California</t>
-  </si>
-  <si>
-    <t>Colorado</t>
-  </si>
-  <si>
-    <t>Connecticut</t>
-  </si>
-  <si>
-    <t>Delaware</t>
-  </si>
-  <si>
-    <t>Florida</t>
-  </si>
-  <si>
-    <t>Georgia</t>
-  </si>
-  <si>
-    <t>Idaho</t>
-  </si>
-  <si>
-    <t>Illinois</t>
-  </si>
-  <si>
-    <t>Indiana</t>
-  </si>
-  <si>
-    <t>Iowa</t>
-  </si>
-  <si>
-    <t>Kansas</t>
-  </si>
-  <si>
-    <t>Kentucky</t>
-  </si>
-  <si>
-    <t>Louisiana</t>
-  </si>
-  <si>
-    <t>Maine</t>
-  </si>
-  <si>
-    <t>Maryland</t>
-  </si>
-  <si>
-    <t>Massachusetts</t>
-  </si>
-  <si>
-    <t>Michigan</t>
-  </si>
-  <si>
-    <t>Minnesota</t>
-  </si>
-  <si>
-    <t>Mississippi</t>
-  </si>
-  <si>
-    <t>Missouri</t>
-  </si>
-  <si>
-    <t>Montana</t>
-  </si>
-  <si>
-    <t>Nebraska</t>
-  </si>
-  <si>
-    <t>Nevada</t>
-  </si>
-  <si>
-    <t>New Hampshire</t>
-  </si>
-  <si>
-    <t>New Jersey</t>
-  </si>
-  <si>
-    <t>New Mexico</t>
-  </si>
-  <si>
-    <t>New York</t>
-  </si>
-  <si>
-    <t>North Carolina</t>
-  </si>
-  <si>
-    <t>North Dakota</t>
-  </si>
-  <si>
-    <t>Ohio</t>
-  </si>
-  <si>
-    <t>Oklahoma</t>
-  </si>
-  <si>
-    <t>Oregon</t>
-  </si>
-  <si>
-    <t>Pennsylvania</t>
-  </si>
-  <si>
-    <t>Rhode Island</t>
-  </si>
-  <si>
-    <t>South Carolina</t>
-  </si>
-  <si>
-    <t>South Dakota</t>
-  </si>
-  <si>
-    <t>Tennessee</t>
-  </si>
-  <si>
-    <t>Texas</t>
-  </si>
-  <si>
-    <t>Utah</t>
-  </si>
-  <si>
-    <t>Vermont</t>
-  </si>
-  <si>
-    <t>Virginia</t>
-  </si>
-  <si>
-    <t>Washington</t>
-  </si>
-  <si>
-    <t>West Virginia</t>
-  </si>
-  <si>
-    <t>Wisconsin</t>
-  </si>
-  <si>
-    <t>Wyoming</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>AK</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>AZ</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>HI</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>KS</t>
+  </si>
+  <si>
+    <t>KY</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>MI</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>ND</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>NJ</t>
+  </si>
+  <si>
+    <t>NM</t>
+  </si>
+  <si>
+    <t>NV</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>OH</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>RI</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>UT</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>VT</t>
+  </si>
+  <si>
+    <t>WA</t>
+  </si>
+  <si>
+    <t>WI</t>
+  </si>
+  <si>
+    <t>WV</t>
+  </si>
+  <si>
+    <t>State</t>
   </si>
 </sst>
 </file>
@@ -201,10 +207,11 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF555555"/>
-      <name val="Georgia"/>
-      <family val="1"/>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="PT Sans"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -230,8 +237,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F034039-973B-394D-99CE-C4869131B1F2}">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="107" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -559,17 +566,20 @@
     <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B1" s="3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="2">
         <v>43831</v>
       </c>
-      <c r="C1" s="3">
+      <c r="C1" s="2">
         <v>43922</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
+    <row r="2" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>56.23</v>
@@ -577,10 +587,13 @@
       <c r="C2" s="1">
         <v>12.59</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>56.49</v>
@@ -588,10 +601,13 @@
       <c r="C3" s="1">
         <v>12.29</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
+      <c r="D3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>59.2</v>
@@ -599,10 +615,13 @@
       <c r="C4" s="1">
         <v>15.36</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>52.23</v>
@@ -610,10 +629,13 @@
       <c r="C5" s="1">
         <v>12.74</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>63.03</v>
@@ -621,10 +643,13 @@
       <c r="C6" s="1">
         <v>19.489999999999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>5</v>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>51.78</v>
@@ -632,10 +657,13 @@
       <c r="C7" s="1">
         <v>9.5299999999999994</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>52.18</v>
@@ -643,10 +671,13 @@
       <c r="C8" s="1">
         <v>12.23</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>7</v>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="B9" s="1">
         <v>52.18</v>
@@ -654,10 +685,13 @@
       <c r="C9" s="1">
         <v>12.23</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>8</v>
+      <c r="D9" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B10" s="1">
         <v>51.36</v>
@@ -665,10 +699,13 @@
       <c r="C10" s="1">
         <v>12.23</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>9</v>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="B11" s="1">
         <v>51.36</v>
@@ -676,10 +713,13 @@
       <c r="C11" s="1">
         <v>12.23</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>10</v>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="B12" s="1">
         <v>54.31</v>
@@ -687,10 +727,13 @@
       <c r="C12" s="1">
         <v>12.74</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>11</v>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="B13" s="1">
         <v>55.74</v>
@@ -698,10 +741,13 @@
       <c r="C13" s="1">
         <v>16.22</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>12</v>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="B14" s="1">
         <v>55.94</v>
@@ -709,10 +755,13 @@
       <c r="C14" s="1">
         <v>16.29</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>13</v>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="B15" s="1">
         <v>54.31</v>
@@ -721,9 +770,9 @@
         <v>12.74</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>14</v>
+    <row r="16" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="B16" s="1">
         <v>53.68</v>
@@ -731,10 +780,13 @@
       <c r="C16" s="1">
         <v>14.4</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>15</v>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="B17" s="1">
         <v>54.12</v>
@@ -742,10 +794,13 @@
       <c r="C17" s="1">
         <v>16.64</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>16</v>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="B18" s="1">
         <v>59.04</v>
@@ -753,10 +808,13 @@
       <c r="C18" s="1">
         <v>16.12</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>17</v>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="B19" s="1">
         <v>52.18</v>
@@ -764,10 +822,13 @@
       <c r="C19" s="1">
         <v>12.23</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>18</v>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="B20" s="1">
         <v>52.18</v>
@@ -775,10 +836,13 @@
       <c r="C20" s="1">
         <v>12.23</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>19</v>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="B21" s="1">
         <v>52.18</v>
@@ -786,10 +850,13 @@
       <c r="C21" s="1">
         <v>12.23</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>20</v>
+      <c r="D21" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="B22" s="1">
         <v>56.54</v>
@@ -798,9 +865,9 @@
         <v>15.73</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>21</v>
+    <row r="23" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B23" s="1">
         <v>54.31</v>
@@ -808,10 +875,13 @@
       <c r="C23" s="1">
         <v>12.74</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>22</v>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B24" s="1">
         <v>56.07</v>
@@ -819,10 +889,13 @@
       <c r="C24" s="1">
         <v>14.14</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>23</v>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="B25" s="1">
         <v>54.31</v>
@@ -830,10 +903,13 @@
       <c r="C25" s="1">
         <v>12.74</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>24</v>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B26" s="1">
         <v>54.31</v>
@@ -841,10 +917,13 @@
       <c r="C26" s="1">
         <v>9.9499999999999993</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>25</v>
+      <c r="D26" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="B27" s="1">
         <v>51.24</v>
@@ -852,10 +931,13 @@
       <c r="C27" s="1">
         <v>11.81</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>26</v>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B28" s="1">
         <v>59.2</v>
@@ -863,10 +945,13 @@
       <c r="C28" s="1">
         <v>15.36</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>27</v>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B29" s="1">
         <v>52.18</v>
@@ -874,10 +959,13 @@
       <c r="C29" s="1">
         <v>12.23</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>28</v>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="B30" s="1">
         <v>52.18</v>
@@ -885,10 +973,13 @@
       <c r="C30" s="1">
         <v>12.23</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>29</v>
+      <c r="D30" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B31" s="1">
         <v>56.55</v>
@@ -896,10 +987,13 @@
       <c r="C31" s="1">
         <v>15.4</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>30</v>
+      <c r="D31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="B32" s="1">
         <v>52.18</v>
@@ -907,10 +1001,13 @@
       <c r="C32" s="1">
         <v>12.23</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
-        <v>31</v>
+      <c r="D32" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="B33" s="1">
         <v>52.18</v>
@@ -918,10 +1015,13 @@
       <c r="C33" s="1">
         <v>12.23</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
-        <v>32</v>
+      <c r="D33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="B34" s="1">
         <v>53.65</v>
@@ -929,10 +1029,13 @@
       <c r="C34" s="1">
         <v>11.76</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>33</v>
+      <c r="D34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="B35" s="1">
         <v>52.77</v>
@@ -940,10 +1043,13 @@
       <c r="C35" s="1">
         <v>13.61</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>34</v>
+      <c r="D35" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="B36" s="1">
         <v>55.78</v>
@@ -951,10 +1057,13 @@
       <c r="C36" s="1">
         <v>14.28</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
-        <v>35</v>
+      <c r="D36" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="B37" s="1">
         <v>59.2</v>
@@ -962,10 +1071,13 @@
       <c r="C37" s="1">
         <v>15.36</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>36</v>
+      <c r="D37" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="B38" s="1">
         <v>51.33</v>
@@ -973,10 +1085,13 @@
       <c r="C38" s="1">
         <v>11.81</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>37</v>
+      <c r="D38" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="B39" s="1">
         <v>52.18</v>
@@ -984,10 +1099,13 @@
       <c r="C39" s="1">
         <v>12.23</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
-        <v>38</v>
+      <c r="D39" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="B40" s="1">
         <v>52.18</v>
@@ -995,10 +1113,13 @@
       <c r="C40" s="1">
         <v>12.23</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
-        <v>39</v>
+      <c r="D40" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="B41" s="1">
         <v>50.88</v>
@@ -1006,10 +1127,13 @@
       <c r="C41" s="1">
         <v>10.050000000000001</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
-        <v>40</v>
+      <c r="D41" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B42" s="1">
         <v>54.31</v>
@@ -1017,10 +1141,13 @@
       <c r="C42" s="1">
         <v>12.74</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
-        <v>41</v>
+      <c r="D42" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="B43" s="1">
         <v>57.63</v>
@@ -1028,10 +1155,13 @@
       <c r="C43" s="1">
         <v>16.25</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
-        <v>42</v>
+      <c r="D43" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="B44" s="1">
         <v>49.02</v>
@@ -1039,10 +1169,13 @@
       <c r="C44" s="1">
         <v>18.690000000000001</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
-        <v>43</v>
+      <c r="D44" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="B45" s="1">
         <v>52.18</v>
@@ -1050,10 +1183,13 @@
       <c r="C45" s="1">
         <v>12.23</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
-        <v>44</v>
+      <c r="D45" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="B46" s="1">
         <v>52.18</v>
@@ -1061,10 +1197,13 @@
       <c r="C46" s="1">
         <v>12.23</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
-        <v>45</v>
+      <c r="D46" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="B47" s="1">
         <v>59.2</v>
@@ -1073,9 +1212,9 @@
         <v>15.36</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
-        <v>46</v>
+    <row r="48" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="B48" s="1">
         <v>51.36</v>
@@ -1084,9 +1223,9 @@
         <v>12.26</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
-        <v>47</v>
+    <row r="49" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="B49" s="1">
         <v>54.31</v>
@@ -1095,9 +1234,9 @@
         <v>12.74</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
-        <v>48</v>
+    <row r="50" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="B50" s="1">
         <v>51.07</v>

</xml_diff>